<commit_message>
Add some documentation to the project
</commit_message>
<xml_diff>
--- a/docs/PIN_Mapping.xlsx
+++ b/docs/PIN_Mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\DUNE_Daphne_v3_AFE\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23D7D4F3-D5E4-44DB-AA47-388988FF2AA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83F01F97-FF03-46A8-8529-F1C42D2379DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="108">
   <si>
     <t>AFE 0</t>
   </si>
@@ -326,6 +326,24 @@
   </si>
   <si>
     <t>BGA Name</t>
+  </si>
+  <si>
+    <t>PL_SCL</t>
+  </si>
+  <si>
+    <t>B44-2</t>
+  </si>
+  <si>
+    <t>PL_SDA</t>
+  </si>
+  <si>
+    <t>B45-2</t>
+  </si>
+  <si>
+    <t>AD11</t>
+  </si>
+  <si>
+    <t>AD10</t>
   </si>
 </sst>
 </file>
@@ -396,7 +414,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -419,11 +437,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -445,6 +515,17 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -663,10 +744,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A3:K20"/>
+  <dimension ref="A3:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -674,7 +755,7 @@
     <col min="1" max="1" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>99</v>
       </c>
@@ -699,7 +780,7 @@
       </c>
       <c r="K3" s="11"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="9" t="s">
         <v>100</v>
@@ -732,7 +813,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="C5" s="1"/>
@@ -745,7 +826,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -764,7 +845,7 @@
       <c r="J6" s="6"/>
       <c r="K6" s="7"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
@@ -783,7 +864,7 @@
       <c r="J7" s="6"/>
       <c r="K7" s="7"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
@@ -818,7 +899,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
@@ -853,77 +934,77 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A10" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="H10" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="I10" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="J10" s="5" t="s">
+      <c r="J10" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="K10" s="4" t="s">
+      <c r="K10" s="15" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:11" s="23" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A11" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H11" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="I11" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="J11" s="5" t="s">
+      <c r="J11" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="K11" s="4" t="s">
+      <c r="K11" s="22" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>43</v>
       </c>
@@ -958,7 +1039,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>54</v>
       </c>
@@ -993,7 +1074,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>65</v>
       </c>
@@ -1028,7 +1109,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>76</v>
       </c>
@@ -1076,7 +1157,7 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>87</v>
       </c>
@@ -1095,7 +1176,7 @@
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>90</v>
       </c>
@@ -1114,7 +1195,7 @@
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>93</v>
       </c>
@@ -1133,24 +1214,75 @@
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
+    <row r="20" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A20" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
+    </row>
+    <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="17"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="17"/>
+    </row>
+    <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17"/>
+      <c r="K22" s="17"/>
+    </row>
+    <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17"/>
+      <c r="K23" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>